<commit_message>
[google.xlsx] update data for browserstack
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/Google/google.xlsx
+++ b/src/test/resources/excelData/Google/google.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\SeleniumFramework\src\test\resources\excelData\Google\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292E4236-D262-4554-8587-536D4A0212B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9928DD88-8E62-4A47-B84E-2D33F8DBD596}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -121,42 +121,9 @@
     <t>IosNativeTest</t>
   </si>
   <si>
-    <t>local</t>
-  </si>
-  <si>
-    <t>desktopChrome</t>
-  </si>
-  <si>
-    <t>desktopSafari</t>
-  </si>
-  <si>
-    <t>desktopFirefox</t>
-  </si>
-  <si>
-    <t>desktopEdge</t>
-  </si>
-  <si>
-    <t>androidChrome</t>
-  </si>
-  <si>
-    <t>androidNative</t>
-  </si>
-  <si>
-    <t>iosSafari</t>
-  </si>
-  <si>
-    <t>iosNative</t>
-  </si>
-  <si>
-    <t>perfecto</t>
-  </si>
-  <si>
     <t>platform</t>
   </si>
   <si>
-    <t>windows 10</t>
-  </si>
-  <si>
     <t>resolution</t>
   </si>
   <si>
@@ -175,21 +142,6 @@
     <t>SystemOption</t>
   </si>
   <si>
-    <t>android</t>
-  </si>
-  <si>
-    <t>iOS</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
-    <t>desktopIe</t>
-  </si>
-  <si>
     <t>AndroidChromeTest2</t>
   </si>
   <si>
@@ -197,6 +149,12 @@
   </si>
   <si>
     <t>monkey</t>
+  </si>
+  <si>
+    <t>com.google.android.apps.docs</t>
+  </si>
+  <si>
+    <t>.drive.startup.StartupActivity</t>
   </si>
 </sst>
 </file>
@@ -322,7 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,6 +313,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -682,10 +641,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -693,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -701,7 +660,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -709,7 +668,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +676,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +684,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +692,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -741,7 +700,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -749,7 +708,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,7 +716,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -765,7 +724,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -773,7 +732,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -784,10 +743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2D1F1-7BA5-4534-88B6-D969E332B0E1}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>14</v>
@@ -855,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>3</v>
@@ -873,7 +832,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>18</v>
@@ -913,21 +872,11 @@
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -948,21 +897,11 @@
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -983,21 +922,11 @@
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="3">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1018,21 +947,11 @@
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1053,15 +972,11 @@
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1082,17 +997,11 @@
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1111,19 +1020,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1145,14 +1048,10 @@
         <v>28</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1162,13 +1061,13 @@
       <c r="M10" s="3"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
       <c r="S10" s="13" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -1177,17 +1076,11 @@
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1208,26 +1101,18 @@
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="M12" s="3"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -1236,6 +1121,17 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>